<commit_message>
edit seo excel file
</commit_message>
<xml_diff>
--- a/SEO/Keywords_Clusters.xlsx
+++ b/SEO/Keywords_Clusters.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Natural Language Understanding</t>
   </si>
   <si>
-    <t xml:space="preserve">Preprocessing</t>
+    <t xml:space="preserve">Text Preprocessing</t>
   </si>
   <si>
     <t xml:space="preserve">Data Cleaning Techniques</t>
@@ -658,31 +658,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -766,7 +766,7 @@
   <dimension ref="A1:C155"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
add crisp messaging code
</commit_message>
<xml_diff>
--- a/SEO/Keywords_Clusters.xlsx
+++ b/SEO/Keywords_Clusters.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="172">
   <si>
     <t xml:space="preserve">Cluster</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sentiment Analysis Tools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">youtube comments sentiment analysis</t>
   </si>
   <si>
     <t xml:space="preserve">Sentiment Analysis Machine Learning</t>
@@ -706,12 +703,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -777,23 +774,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C155"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="18.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="58.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="58.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="59.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="1" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -988,16 +985,13 @@
       <c r="B23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="24" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1005,7 +999,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1013,7 +1007,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,7 +1015,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1029,7 +1023,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1037,7 +1031,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1045,7 +1039,7 @@
         <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1053,7 +1047,7 @@
         <v>24</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,7 +1055,7 @@
         <v>24</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1069,7 +1063,7 @@
         <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1077,7 +1071,7 @@
         <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1085,7 +1079,7 @@
         <v>24</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,7 +1087,7 @@
         <v>24</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1101,7 +1095,7 @@
         <v>24</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1109,7 +1103,7 @@
         <v>24</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1117,7 +1111,7 @@
         <v>24</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1125,7 +1119,7 @@
         <v>24</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1133,7 +1127,7 @@
         <v>24</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1141,7 +1135,7 @@
         <v>24</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1149,912 +1143,912 @@
         <v>24</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="C121" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B122" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B123" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B134" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B147" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>